<commit_message>
estimate changed for chinimaya mam
</commit_message>
<xml_diff>
--- a/ofc/estimates/nabin sir/khulaltar sankalpa measurement.xlsx
+++ b/ofc/estimates/nabin sir/khulaltar sankalpa measurement.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Measurement" sheetId="6" state="hidden" r:id="rId1"/>
-    <sheet name="measure quantity" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="Measurement" sheetId="6" r:id="rId1"/>
+    <sheet name="measure quantity" sheetId="7" r:id="rId2"/>
     <sheet name="measure quantity (2)" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="final" sheetId="9" r:id="rId4"/>
   </sheets>
@@ -55,7 +55,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">final!$A$1:$K$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'measure quantity'!$A$1:$K$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'measure quantity (2)'!$A$1:$K$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Measurement!$A$2:$N$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Measurement!$A$2:$P$67</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">final!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'measure quantity'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'measure quantity (2)'!$1:$8</definedName>
@@ -464,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -589,6 +589,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1395,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:X66"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23:N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,72 +1413,78 @@
     <col min="4" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
-    <col min="10" max="11" width="8.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="31" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="31" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="60" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="60"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="P2" s="62"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="60" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="60"/>
-    </row>
-    <row r="4" spans="1:22" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="62"/>
+    </row>
+    <row r="4" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1487,28 +1497,30 @@
       <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="61"/>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
       <c r="J4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>32</v>
       </c>
@@ -1524,18 +1536,20 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="14"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="14"/>
+      <c r="R5" s="19"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-    </row>
-    <row r="6" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+    </row>
+    <row r="6" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>16</v>
@@ -1557,21 +1571,23 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="15">
-        <f t="shared" ref="L6" si="0">PRODUCT(C6:J6)</f>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15">
+        <f t="shared" ref="N6" si="0">PRODUCT(C6:J6)</f>
         <v>31.872642176780758</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="14"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="14"/>
+      <c r="R6" s="19"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-    </row>
-    <row r="7" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+    </row>
+    <row r="7" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="20" t="s">
         <v>10</v>
@@ -1585,16 +1601,18 @@
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
-      <c r="L7" s="24">
-        <f>0*SUM(L6:L6)</f>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="24">
+        <f>0*SUM(N6:N6)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="O7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="25"/>
-    </row>
-    <row r="8" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="25"/>
+    </row>
+    <row r="8" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="20" t="s">
         <v>13</v>
@@ -1608,11 +1626,13 @@
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="25"/>
-    </row>
-    <row r="9" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="25"/>
+    </row>
+    <row r="9" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="20"/>
       <c r="C9" s="23"/>
@@ -1624,11 +1644,13 @@
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="25"/>
-    </row>
-    <row r="10" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="25"/>
+    </row>
+    <row r="10" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>33</v>
       </c>
@@ -1644,11 +1666,13 @@
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="25"/>
-    </row>
-    <row r="11" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="25"/>
+    </row>
+    <row r="11" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
         <v>16</v>
@@ -1668,21 +1692,23 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="15">
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15">
         <f>PRODUCT(C11:J11)</f>
         <v>19.455653764096311</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="14"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="14"/>
+      <c r="R11" s="19"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-    </row>
-    <row r="12" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+    </row>
+    <row r="12" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="20" t="s">
         <v>10</v>
@@ -1696,16 +1722,18 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
-      <c r="L12" s="24">
-        <f>0*SUM(L11:L11)</f>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="24">
+        <f>0*SUM(N11:N11)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="O12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="25"/>
-    </row>
-    <row r="13" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="25"/>
+    </row>
+    <row r="13" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="20" t="s">
         <v>13</v>
@@ -1719,11 +1747,13 @@
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="25"/>
-    </row>
-    <row r="14" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="20"/>
       <c r="C14" s="23"/>
@@ -1735,11 +1765,13 @@
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="25"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>34</v>
       </c>
@@ -1755,11 +1787,13 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="25"/>
-    </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="25"/>
+    </row>
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="20" t="s">
         <v>19</v>
@@ -1775,14 +1809,16 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
-      <c r="L16" s="15">
-        <f t="shared" ref="L16" si="1">PRODUCT(C16:J16)</f>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15">
+        <f t="shared" ref="N16" si="1">PRODUCT(C16:J16)</f>
         <v>4</v>
       </c>
-      <c r="M16" s="26"/>
-      <c r="N16" s="25"/>
-    </row>
-    <row r="17" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="26"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="20" t="s">
         <v>10</v>
@@ -1796,16 +1832,18 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
-      <c r="L17" s="24">
-        <f>0*SUM(L16)</f>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="24">
+        <f>0*SUM(N16)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="O17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="25"/>
-    </row>
-    <row r="18" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="25"/>
+    </row>
+    <row r="18" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="20" t="s">
         <v>13</v>
@@ -1819,11 +1857,13 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="25"/>
-    </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="25"/>
+    </row>
+    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="21"/>
       <c r="C19" s="23"/>
@@ -1835,11 +1875,13 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="25"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="25"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>1</v>
       </c>
@@ -1859,11 +1901,13 @@
       <c r="I20" s="24"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="25"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="25"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="36" t="s">
         <v>26</v>
@@ -1877,11 +1921,13 @@
       <c r="I21" s="24"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="25"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="25"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="11" t="s">
         <v>23</v>
@@ -1900,11 +1946,16 @@
         <v>0.9</v>
       </c>
       <c r="K22" s="15"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="25"/>
-    </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="15">
+        <f>J22-0.15</f>
+        <v>0.75</v>
+      </c>
+      <c r="M22" s="15"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="25"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>29</v>
@@ -1940,18 +1991,29 @@
         <f>(J22+J23)/2</f>
         <v>0.9</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="14"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="L23" s="15">
+        <f>J23-0.15</f>
+        <v>0.75</v>
+      </c>
+      <c r="M23" s="53">
+        <f>(L22+L23)/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="N23" s="15">
+        <f>M23*I23*D23</f>
+        <v>1.4175</v>
+      </c>
+      <c r="O23" s="16"/>
+      <c r="P23" s="14"/>
+      <c r="R23" s="19"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-    </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+    </row>
+    <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>28</v>
@@ -1987,18 +2049,29 @@
         <f>(J23+J24)/2</f>
         <v>0.875</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="14"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
+      <c r="L24" s="15">
+        <f>J24-0.15</f>
+        <v>0.7</v>
+      </c>
+      <c r="M24" s="53">
+        <f>(L23+L24)/2</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="N24" s="15">
+        <f t="shared" ref="N24:N64" si="2">M24*I24*D24</f>
+        <v>1.3865624999999999</v>
+      </c>
+      <c r="O24" s="16"/>
+      <c r="P24" s="14"/>
+      <c r="R24" s="19"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-    </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12"/>
@@ -2011,17 +2084,19 @@
       <c r="J25" s="14"/>
       <c r="K25" s="54"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="14"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="14"/>
+      <c r="R25" s="19"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-    </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="36" t="s">
         <v>27</v>
@@ -2036,17 +2111,19 @@
       <c r="J26" s="14"/>
       <c r="K26" s="54"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="14"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="14"/>
+      <c r="R26" s="19"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="11" t="s">
         <v>23</v>
@@ -2066,11 +2143,16 @@
         <v>0.5</v>
       </c>
       <c r="K27" s="53"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="25"/>
-    </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="15">
+        <f>J27-0.15</f>
+        <v>0.35</v>
+      </c>
+      <c r="M27" s="53"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="25"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
         <v>30</v>
@@ -2104,18 +2186,29 @@
         <f>(J27+J28)/2</f>
         <v>0.45499999999999996</v>
       </c>
-      <c r="L28" s="15"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="14"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
+      <c r="L28" s="15">
+        <f>J28-0.15</f>
+        <v>0.26</v>
+      </c>
+      <c r="M28" s="53">
+        <f>(L27+L28)/2</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="N28" s="15">
+        <f t="shared" si="2"/>
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="O28" s="16"/>
+      <c r="P28" s="14"/>
+      <c r="R28" s="19"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-    </row>
-    <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+    </row>
+    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
@@ -2128,17 +2221,19 @@
       <c r="J29" s="14"/>
       <c r="K29" s="54"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="14"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="14"/>
+      <c r="R29" s="19"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-    </row>
-    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="36" t="s">
         <v>31</v>
@@ -2153,17 +2248,19 @@
       <c r="J30" s="14"/>
       <c r="K30" s="54"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="14"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="14"/>
+      <c r="R30" s="19"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="11" t="s">
         <v>23</v>
@@ -2183,11 +2280,16 @@
         <v>0.9</v>
       </c>
       <c r="K31" s="53"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="25"/>
-    </row>
-    <row r="32" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L31" s="15">
+        <f>J31-0.15</f>
+        <v>0.75</v>
+      </c>
+      <c r="M31" s="53"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="25"/>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>32</v>
@@ -2221,18 +2323,29 @@
         <f>(J31+J32)/2</f>
         <v>1.075</v>
       </c>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="14"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
+      <c r="L32" s="15">
+        <f>J32-0.15</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M32" s="53">
+        <f>(L31+L32)/2</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="N32" s="15">
+        <f t="shared" si="2"/>
+        <v>3.4217599999999999</v>
+      </c>
+      <c r="O32" s="16"/>
+      <c r="P32" s="14"/>
+      <c r="R32" s="19"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-    </row>
-    <row r="33" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+    </row>
+    <row r="33" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>33</v>
@@ -2246,14 +2359,14 @@
         <v>0.52</v>
       </c>
       <c r="F33" s="53">
-        <f t="shared" ref="F33:F34" si="2">(E32+E33)/2</f>
+        <f t="shared" ref="F33:F34" si="3">(E32+E33)/2</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="G33" s="14">
         <v>0.7</v>
       </c>
       <c r="H33" s="53">
-        <f t="shared" ref="H33:H34" si="3">(G32+G33)/2</f>
+        <f t="shared" ref="H33:H34" si="4">(G32+G33)/2</f>
         <v>0.7</v>
       </c>
       <c r="I33" s="53">
@@ -2264,21 +2377,32 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="K33" s="53">
-        <f t="shared" ref="K33:K34" si="4">(J32+J33)/2</f>
+        <f>(J32+J33)/2</f>
         <v>1.2</v>
       </c>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="14"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
+      <c r="L33" s="15">
+        <f>J33-0.15</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="M33" s="53">
+        <f>(L32+L33)/2</f>
+        <v>1.05</v>
+      </c>
+      <c r="N33" s="15">
+        <f t="shared" si="2"/>
+        <v>3.9374999999999996</v>
+      </c>
+      <c r="O33" s="16"/>
+      <c r="P33" s="14"/>
+      <c r="R33" s="19"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-    </row>
-    <row r="34" spans="1:22" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+    </row>
+    <row r="34" spans="1:24" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="11" t="s">
         <v>34</v>
@@ -2292,14 +2416,14 @@
         <v>0.54</v>
       </c>
       <c r="F34" s="53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.53</v>
       </c>
       <c r="G34" s="14">
         <v>0.7</v>
       </c>
       <c r="H34" s="53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
       <c r="I34" s="53">
@@ -2310,21 +2434,32 @@
         <v>0.9</v>
       </c>
       <c r="K34" s="53">
-        <f t="shared" si="4"/>
+        <f>(J33+J34)/2</f>
         <v>1.0249999999999999</v>
       </c>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="14"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
+      <c r="L34" s="15">
+        <f>J34-0.15</f>
+        <v>0.75</v>
+      </c>
+      <c r="M34" s="53">
+        <f>(L33+L34)/2</f>
+        <v>0.875</v>
+      </c>
+      <c r="N34" s="15">
+        <f t="shared" si="2"/>
+        <v>3.4978125000000007</v>
+      </c>
+      <c r="O34" s="16"/>
+      <c r="P34" s="14"/>
+      <c r="R34" s="19"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-    </row>
-    <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+    </row>
+    <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="12"/>
@@ -2337,17 +2472,19 @@
       <c r="J35" s="14"/>
       <c r="K35" s="54"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="14"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="14"/>
+      <c r="R35" s="19"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-    </row>
-    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+    </row>
+    <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="36" t="s">
         <v>46</v>
@@ -2362,17 +2499,19 @@
       <c r="J36" s="14"/>
       <c r="K36" s="54"/>
       <c r="L36" s="15"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="14"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="14"/>
+      <c r="R36" s="19"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="11" t="s">
         <v>23</v>
@@ -2393,11 +2532,16 @@
         <v>1.8</v>
       </c>
       <c r="K37" s="53"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="25"/>
-    </row>
-    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L37" s="15">
+        <f>J37-0.15</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="M37" s="53"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="25"/>
+    </row>
+    <row r="38" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
         <v>35</v>
@@ -2431,18 +2575,29 @@
         <f>(J37+J38)/2</f>
         <v>1.8</v>
       </c>
-      <c r="L38" s="15"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="14"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+      <c r="L38" s="15">
+        <f>J38-0.15</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="M38" s="53">
+        <f>(L37+L38)/2</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="N38" s="15">
+        <f t="shared" si="2"/>
+        <v>5.3625000000000007</v>
+      </c>
+      <c r="O38" s="16"/>
+      <c r="P38" s="14"/>
+      <c r="R38" s="19"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-    </row>
-    <row r="39" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+    </row>
+    <row r="39" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="11" t="s">
         <v>36</v>
@@ -2473,21 +2628,32 @@
         <v>1.45</v>
       </c>
       <c r="K39" s="53">
-        <f t="shared" ref="K39:K42" si="7">(J38+J39)/2</f>
+        <f>(J38+J39)/2</f>
         <v>1.625</v>
       </c>
-      <c r="L39" s="15"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="14"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
+      <c r="L39" s="15">
+        <f>J39-0.15</f>
+        <v>1.3</v>
+      </c>
+      <c r="M39" s="53">
+        <f>(L38+L39)/2</f>
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="N39" s="15">
+        <f t="shared" si="2"/>
+        <v>4.7937500000000002</v>
+      </c>
+      <c r="O39" s="16"/>
+      <c r="P39" s="14"/>
+      <c r="R39" s="19"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-    </row>
-    <row r="40" spans="1:22" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+    </row>
+    <row r="40" spans="1:24" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
         <v>37</v>
@@ -2518,21 +2684,32 @@
         <v>1.25</v>
       </c>
       <c r="K40" s="53">
-        <f t="shared" si="7"/>
+        <f>(J39+J40)/2</f>
         <v>1.35</v>
       </c>
-      <c r="L40" s="15"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="14"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="L40" s="15">
+        <f>J40-0.15</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M40" s="53">
+        <f>(L39+L40)/2</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="N40" s="15">
+        <f t="shared" si="2"/>
+        <v>3.9000000000000008</v>
+      </c>
+      <c r="O40" s="16"/>
+      <c r="P40" s="14"/>
+      <c r="R40" s="19"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-    </row>
-    <row r="41" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+    </row>
+    <row r="41" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11" t="s">
         <v>38</v>
@@ -2563,21 +2740,32 @@
         <v>1.4</v>
       </c>
       <c r="K41" s="53">
-        <f t="shared" si="7"/>
+        <f>(J40+J41)/2</f>
         <v>1.325</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="14"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
+      <c r="L41" s="15">
+        <f>J41-0.15</f>
+        <v>1.25</v>
+      </c>
+      <c r="M41" s="53">
+        <f>(L40+L41)/2</f>
+        <v>1.175</v>
+      </c>
+      <c r="N41" s="15">
+        <f t="shared" si="2"/>
+        <v>3.8187500000000001</v>
+      </c>
+      <c r="O41" s="16"/>
+      <c r="P41" s="14"/>
+      <c r="R41" s="19"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-    </row>
-    <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+    </row>
+    <row r="42" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
         <v>39</v>
@@ -2608,21 +2796,32 @@
         <v>1.25</v>
       </c>
       <c r="K42" s="53">
-        <f t="shared" si="7"/>
+        <f>(J41+J42)/2</f>
         <v>1.325</v>
       </c>
-      <c r="L42" s="15"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="14"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
+      <c r="L42" s="15">
+        <f>J42-0.15</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M42" s="53">
+        <f>(L41+L42)/2</f>
+        <v>1.175</v>
+      </c>
+      <c r="N42" s="15">
+        <f t="shared" si="2"/>
+        <v>1.451125</v>
+      </c>
+      <c r="O42" s="16"/>
+      <c r="P42" s="14"/>
+      <c r="R42" s="19"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-    </row>
-    <row r="43" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+    </row>
+    <row r="43" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="12"/>
@@ -2635,17 +2834,19 @@
       <c r="J43" s="14"/>
       <c r="K43" s="54"/>
       <c r="L43" s="15"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="14"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="14"/>
+      <c r="R43" s="19"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-    </row>
-    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+    </row>
+    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="36" t="s">
         <v>47</v>
@@ -2660,17 +2861,19 @@
       <c r="J44" s="14"/>
       <c r="K44" s="54"/>
       <c r="L44" s="15"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="14"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="M44" s="54"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="14"/>
+      <c r="R44" s="19"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="11" t="s">
         <v>23</v>
@@ -2690,11 +2893,16 @@
         <v>2.1</v>
       </c>
       <c r="K45" s="53"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="25"/>
-    </row>
-    <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L45" s="15">
+        <f>J45-0.15</f>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="M45" s="53"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="25"/>
+    </row>
+    <row r="46" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11" t="s">
         <v>40</v>
@@ -2728,18 +2936,29 @@
         <f>(J45+J46)/2</f>
         <v>2.1</v>
       </c>
-      <c r="L46" s="15"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="14"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="L46" s="15">
+        <f>J46-0.15</f>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="M46" s="53">
+        <f>(L45+L46)/2</f>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="N46" s="15">
+        <f t="shared" si="2"/>
+        <v>17.472000000000001</v>
+      </c>
+      <c r="O46" s="16"/>
+      <c r="P46" s="14"/>
+      <c r="R46" s="19"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-    </row>
-    <row r="47" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+    </row>
+    <row r="47" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
@@ -2752,17 +2971,19 @@
       <c r="J47" s="14"/>
       <c r="K47" s="54"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="14"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="14"/>
+      <c r="R47" s="19"/>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-    </row>
-    <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+    </row>
+    <row r="48" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="36" t="s">
         <v>48</v>
@@ -2777,17 +2998,19 @@
       <c r="J48" s="14"/>
       <c r="K48" s="54"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="14"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
+      <c r="M48" s="54"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="14"/>
+      <c r="R48" s="19"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
       <c r="B49" s="11" t="s">
         <v>23</v>
@@ -2807,11 +3030,16 @@
         <v>1.5</v>
       </c>
       <c r="K49" s="53"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="25"/>
-    </row>
-    <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L49" s="15">
+        <f>J49-0.15</f>
+        <v>1.35</v>
+      </c>
+      <c r="M49" s="53"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="25"/>
+    </row>
+    <row r="50" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="11" t="s">
         <v>35</v>
@@ -2845,18 +3073,29 @@
         <f>(J49+J50)/2</f>
         <v>1.5249999999999999</v>
       </c>
-      <c r="L50" s="15"/>
-      <c r="M50" s="16"/>
-      <c r="N50" s="14"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+      <c r="L50" s="15">
+        <f>J50-0.15</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="M50" s="53">
+        <f>(L49+L50)/2</f>
+        <v>1.375</v>
+      </c>
+      <c r="N50" s="15">
+        <f t="shared" si="2"/>
+        <v>4.1250000000000009</v>
+      </c>
+      <c r="O50" s="16"/>
+      <c r="P50" s="14"/>
+      <c r="R50" s="19"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="19"/>
-    </row>
-    <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+    </row>
+    <row r="51" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="11" t="s">
         <v>36</v>
@@ -2869,14 +3108,14 @@
         <v>0.4</v>
       </c>
       <c r="F51" s="53">
-        <f t="shared" ref="F51:F52" si="8">(E50+E51)/2</f>
+        <f t="shared" ref="F51:F52" si="7">(E50+E51)/2</f>
         <v>0.4</v>
       </c>
       <c r="G51" s="14">
         <v>0.8</v>
       </c>
       <c r="H51" s="53">
-        <f t="shared" ref="H51:H52" si="9">(G50+G51)/2</f>
+        <f t="shared" ref="H51:H52" si="8">(G50+G51)/2</f>
         <v>0.8</v>
       </c>
       <c r="I51" s="53">
@@ -2887,21 +3126,32 @@
         <v>1.4</v>
       </c>
       <c r="K51" s="53">
-        <f t="shared" ref="K51:K52" si="10">(J50+J51)/2</f>
+        <f>(J50+J51)/2</f>
         <v>1.4750000000000001</v>
       </c>
-      <c r="L51" s="15"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="14"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
+      <c r="L51" s="15">
+        <f>J51-0.15</f>
+        <v>1.25</v>
+      </c>
+      <c r="M51" s="53">
+        <f>(L50+L51)/2</f>
+        <v>1.3250000000000002</v>
+      </c>
+      <c r="N51" s="15">
+        <f t="shared" si="2"/>
+        <v>3.9750000000000014</v>
+      </c>
+      <c r="O51" s="16"/>
+      <c r="P51" s="14"/>
+      <c r="R51" s="19"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="19"/>
-    </row>
-    <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="19"/>
+      <c r="X51" s="19"/>
+    </row>
+    <row r="52" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
         <v>42</v>
@@ -2914,14 +3164,14 @@
         <v>0.4</v>
       </c>
       <c r="F52" s="53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.4</v>
       </c>
       <c r="G52" s="14">
         <v>0.8</v>
       </c>
       <c r="H52" s="53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
       <c r="I52" s="53">
@@ -2932,21 +3182,32 @@
         <v>1.2</v>
       </c>
       <c r="K52" s="53">
-        <f t="shared" si="10"/>
+        <f>(J51+J52)/2</f>
         <v>1.2999999999999998</v>
       </c>
-      <c r="L52" s="15"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="14"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
+      <c r="L52" s="15">
+        <f>J52-0.15</f>
+        <v>1.05</v>
+      </c>
+      <c r="M52" s="53">
+        <f>(L51+L52)/2</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N52" s="15">
+        <f t="shared" si="2"/>
+        <v>3.1739999999999999</v>
+      </c>
+      <c r="O52" s="16"/>
+      <c r="P52" s="14"/>
+      <c r="R52" s="19"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="19"/>
-    </row>
-    <row r="53" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19"/>
+    </row>
+    <row r="53" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
@@ -2959,17 +3220,22 @@
       <c r="J53" s="14"/>
       <c r="K53" s="54"/>
       <c r="L53" s="15"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="14"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="M53" s="54"/>
+      <c r="N53" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O53" s="16"/>
+      <c r="P53" s="14"/>
+      <c r="R53" s="19"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="19"/>
-    </row>
-    <row r="54" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19"/>
+    </row>
+    <row r="54" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="36" t="s">
         <v>49</v>
@@ -2984,17 +3250,22 @@
       <c r="J54" s="14"/>
       <c r="K54" s="54"/>
       <c r="L54" s="15"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="14"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O54" s="16"/>
+      <c r="P54" s="14"/>
+      <c r="R54" s="19"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
-      <c r="U54" s="19"/>
-      <c r="V54" s="19"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="19"/>
+      <c r="X54" s="19"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
       <c r="B55" s="11" t="s">
         <v>23</v>
@@ -3014,11 +3285,19 @@
         <v>1.2</v>
       </c>
       <c r="K55" s="53"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
-      <c r="N55" s="25"/>
-    </row>
-    <row r="56" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L55" s="15">
+        <f>J55-0.15</f>
+        <v>1.05</v>
+      </c>
+      <c r="M55" s="53"/>
+      <c r="N55" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O55" s="26"/>
+      <c r="P55" s="25"/>
+    </row>
+    <row r="56" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="11" t="s">
         <v>43</v>
@@ -3052,18 +3331,29 @@
         <f>(J55+J56)/2</f>
         <v>1.2</v>
       </c>
-      <c r="L56" s="15"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="14"/>
-      <c r="P56" s="19"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
+      <c r="L56" s="15">
+        <f>J56-0.15</f>
+        <v>1.05</v>
+      </c>
+      <c r="M56" s="53">
+        <f>(L55+L56)/2</f>
+        <v>1.05</v>
+      </c>
+      <c r="N56" s="15">
+        <f t="shared" si="2"/>
+        <v>7.7385000000000019</v>
+      </c>
+      <c r="O56" s="16"/>
+      <c r="P56" s="14"/>
+      <c r="R56" s="19"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
-      <c r="U56" s="19"/>
-      <c r="V56" s="19"/>
-    </row>
-    <row r="57" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="19"/>
+      <c r="X56" s="19"/>
+    </row>
+    <row r="57" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="11"/>
       <c r="C57" s="12"/>
@@ -3076,17 +3366,19 @@
       <c r="J57" s="14"/>
       <c r="K57" s="54"/>
       <c r="L57" s="15"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="14"/>
-      <c r="P57" s="19"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="14"/>
+      <c r="R57" s="19"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
-      <c r="U57" s="19"/>
-      <c r="V57" s="19"/>
-    </row>
-    <row r="58" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="19"/>
+      <c r="X57" s="19"/>
+    </row>
+    <row r="58" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="36" t="s">
         <v>50</v>
@@ -3101,17 +3393,19 @@
       <c r="J58" s="14"/>
       <c r="K58" s="54"/>
       <c r="L58" s="15"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="14"/>
-      <c r="P58" s="19"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+      <c r="M58" s="54"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="14"/>
+      <c r="R58" s="19"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
-      <c r="U58" s="19"/>
-      <c r="V58" s="19"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="19"/>
+      <c r="X58" s="19"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="11" t="s">
         <v>23</v>
@@ -3131,11 +3425,16 @@
         <v>1</v>
       </c>
       <c r="K59" s="53"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="25"/>
-    </row>
-    <row r="60" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L59" s="15">
+        <f>J59-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="M59" s="53"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="26"/>
+      <c r="P59" s="25"/>
+    </row>
+    <row r="60" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="11" t="s">
         <v>44</v>
@@ -3169,18 +3468,29 @@
         <f>(J59+J60)/2</f>
         <v>1</v>
       </c>
-      <c r="L60" s="15"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="14"/>
-      <c r="P60" s="19"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
+      <c r="L60" s="15">
+        <f>J60-0.15</f>
+        <v>0.85</v>
+      </c>
+      <c r="M60" s="53">
+        <f>(L59+L60)/2</f>
+        <v>0.85</v>
+      </c>
+      <c r="N60" s="15">
+        <f t="shared" si="2"/>
+        <v>0.86827500000000002</v>
+      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="14"/>
+      <c r="R60" s="19"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
-      <c r="U60" s="19"/>
-      <c r="V60" s="19"/>
-    </row>
-    <row r="61" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="19"/>
+      <c r="X60" s="19"/>
+    </row>
+    <row r="61" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="12"/>
@@ -3193,17 +3503,19 @@
       <c r="J61" s="14"/>
       <c r="K61" s="54"/>
       <c r="L61" s="15"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="14"/>
-      <c r="P61" s="19"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="14"/>
+      <c r="R61" s="19"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="19"/>
-    </row>
-    <row r="62" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="19"/>
+      <c r="X61" s="19"/>
+    </row>
+    <row r="62" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="36" t="s">
         <v>51</v>
@@ -3218,17 +3530,19 @@
       <c r="J62" s="14"/>
       <c r="K62" s="54"/>
       <c r="L62" s="15"/>
-      <c r="M62" s="16"/>
-      <c r="N62" s="14"/>
-      <c r="P62" s="19"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="M62" s="54"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="14"/>
+      <c r="R62" s="19"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
-      <c r="U62" s="19"/>
-      <c r="V62" s="19"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="19"/>
+      <c r="X62" s="19"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
       <c r="B63" s="11" t="s">
         <v>23</v>
@@ -3248,11 +3562,16 @@
         <v>1.2</v>
       </c>
       <c r="K63" s="53"/>
-      <c r="L63" s="26"/>
-      <c r="M63" s="26"/>
-      <c r="N63" s="25"/>
-    </row>
-    <row r="64" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L63" s="15">
+        <f>J63-0.15</f>
+        <v>1.05</v>
+      </c>
+      <c r="M63" s="53"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="26"/>
+      <c r="P63" s="25"/>
+    </row>
+    <row r="64" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="11" t="s">
         <v>45</v>
@@ -3262,11 +3581,11 @@
         <v>6.4</v>
       </c>
       <c r="E64" s="13">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="F64" s="53">
         <f>(E63+E64)/2</f>
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="G64" s="14">
         <v>0.7</v>
@@ -3277,7 +3596,7 @@
       </c>
       <c r="I64" s="53">
         <f>(F64+H64)/2</f>
-        <v>0.625</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J64" s="14">
         <v>1.2</v>
@@ -3286,18 +3605,29 @@
         <f>(J63+J64)/2</f>
         <v>1.2</v>
       </c>
-      <c r="L64" s="15"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="14"/>
-      <c r="P64" s="19"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
+      <c r="L64" s="15">
+        <f>J64-0.15</f>
+        <v>1.05</v>
+      </c>
+      <c r="M64" s="53">
+        <f>(L63+L64)/2</f>
+        <v>1.05</v>
+      </c>
+      <c r="N64" s="15">
+        <f t="shared" si="2"/>
+        <v>3.6960000000000011</v>
+      </c>
+      <c r="O64" s="16"/>
+      <c r="P64" s="14"/>
+      <c r="R64" s="19"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
-      <c r="U64" s="19"/>
-      <c r="V64" s="19"/>
-    </row>
-    <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="19"/>
+      <c r="X64" s="19"/>
+    </row>
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22"/>
       <c r="B65" s="20"/>
       <c r="C65" s="23"/>
@@ -3309,11 +3639,13 @@
       <c r="I65" s="15"/>
       <c r="J65" s="15"/>
       <c r="K65" s="15"/>
-      <c r="L65" s="26"/>
-      <c r="M65" s="26"/>
-      <c r="N65" s="25"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="26"/>
+      <c r="O65" s="26"/>
+      <c r="P65" s="25"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
       <c r="B66" s="27" t="s">
         <v>20</v>
@@ -3327,18 +3659,20 @@
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
-      <c r="L66" s="18"/>
-      <c r="M66" s="18"/>
-      <c r="N66" s="25"/>
+      <c r="L66" s="29"/>
+      <c r="M66" s="29"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3356,8 +3690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3380,113 +3714,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="62" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -3842,12 +4176,12 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F21" s="53">
-        <f>Measurement!K56</f>
-        <v>1.2</v>
+        <f>Measurement!K46</f>
+        <v>2.1</v>
       </c>
       <c r="G21" s="43">
         <f t="shared" si="0"/>
-        <v>8.4480000000000004</v>
+        <v>14.784000000000002</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="17"/>
@@ -3995,7 +4329,7 @@
       </c>
       <c r="E27" s="53">
         <f>Measurement!I64</f>
-        <v>0.625</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F27" s="53">
         <f>Measurement!K64</f>
@@ -4003,7 +4337,7 @@
       </c>
       <c r="G27" s="43">
         <f t="shared" si="0"/>
-        <v>4.8</v>
+        <v>4.2240000000000002</v>
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="17"/>
@@ -4089,8 +4423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F27"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,113 +4447,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="62" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -4792,8 +5126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4816,113 +5150,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="62" t="s">
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -5017,7 +5351,7 @@
         <v>0.875</v>
       </c>
       <c r="G11" s="43">
-        <f t="shared" ref="G11:G27" si="0">PRODUCT(C11:F11)</f>
+        <f t="shared" ref="G11:G26" si="0">PRODUCT(C11:F11)</f>
         <v>1.6734374999999999</v>
       </c>
       <c r="H11" s="40"/>
@@ -5261,11 +5595,11 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F21" s="53">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
       <c r="G21" s="43">
         <f t="shared" si="0"/>
-        <v>8.4480000000000004</v>
+        <v>14.784000000000002</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="17"/>
@@ -5440,7 +5774,7 @@
       <c r="F29" s="29"/>
       <c r="G29" s="47">
         <f>SUM(G10:G27)</f>
-        <v>76.114390000000014</v>
+        <v>82.450390000000013</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>65</v>

</xml_diff>